<commit_message>
redrafted ERD and updated Readme
</commit_message>
<xml_diff>
--- a/assets/Project 2 Planning.xlsx
+++ b/assets/Project 2 Planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1165,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF41"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B18" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="V2" workbookViewId="0">
+      <selection activeCell="X4" sqref="X4:AB7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
added public and private routes, routes mounted and functional
</commit_message>
<xml_diff>
--- a/assets/Project 2 Planning.xlsx
+++ b/assets/Project 2 Planning.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="164">
   <si>
     <t xml:space="preserve">Unit 2 Project </t>
   </si>
@@ -500,6 +500,18 @@
   </si>
   <si>
     <t>https://css-tricks.com/snippets/css/a-guide-to-flexbox/</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/places/web-service/autocomplete</t>
+  </si>
+  <si>
+    <t>Google API Autocompletion</t>
+  </si>
+  <si>
+    <t>http://guides.rubyonrails.org/association_basics.html</t>
+  </si>
+  <si>
+    <t>Relationships tables</t>
   </si>
 </sst>
 </file>
@@ -1163,10 +1175,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF41"/>
+  <dimension ref="A1:AF45"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="V2" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4:AB7"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="E11" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2342,44 +2354,14 @@
       </c>
     </row>
     <row r="26" spans="1:28">
-      <c r="A26" t="s">
-        <v>137</v>
-      </c>
-      <c r="K26" t="s">
-        <v>49</v>
-      </c>
-      <c r="L26" t="s">
-        <v>45</v>
-      </c>
-      <c r="M26" t="s">
-        <v>49</v>
-      </c>
-      <c r="O26" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="P26">
-        <f>SUM(P5:P25)</f>
-        <v>31</v>
-      </c>
-      <c r="Q26" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="S26" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="U26" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="X26" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>127</v>
-      </c>
+      <c r="O26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="U26" s="2"/>
     </row>
     <row r="27" spans="1:28">
-      <c r="A27" s="4" t="s">
-        <v>138</v>
+      <c r="G27" t="s">
+        <v>163</v>
       </c>
       <c r="O27" s="2"/>
       <c r="Q27" s="2"/>
@@ -2388,97 +2370,163 @@
     </row>
     <row r="28" spans="1:28">
       <c r="A28" t="s">
-        <v>134</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="G28" t="s">
+        <v>162</v>
+      </c>
+      <c r="O28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="U28" s="2"/>
     </row>
     <row r="29" spans="1:28">
-      <c r="A29" s="4" t="s">
-        <v>140</v>
-      </c>
+      <c r="A29" t="s">
+        <v>160</v>
+      </c>
+      <c r="O29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="U29" s="2"/>
     </row>
     <row r="30" spans="1:28">
-      <c r="A30" s="5" t="s">
-        <v>135</v>
+      <c r="A30" t="s">
+        <v>137</v>
+      </c>
+      <c r="K30" t="s">
+        <v>49</v>
+      </c>
+      <c r="L30" t="s">
+        <v>45</v>
+      </c>
+      <c r="M30" t="s">
+        <v>49</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="P30">
+        <f>SUM(P5:P25)</f>
+        <v>31</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="S30" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U30" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="X30" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:28">
       <c r="A31" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="O31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="U31" s="2"/>
+    </row>
+    <row r="32" spans="1:28">
+      <c r="A32" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="7" t="s">
+    <row r="37" spans="1:7">
+      <c r="A37" s="7" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="8" t="s">
+    <row r="39" spans="1:7">
+      <c r="A39" s="8" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="60">
-      <c r="A36" s="6" t="s">
+    <row r="40" spans="1:7" ht="60">
+      <c r="A40" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B40" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G40" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="5" t="s">
+    <row r="41" spans="1:7">
+      <c r="A41" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B41" t="s">
         <v>144</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C41" t="s">
         <v>142</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G41" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
-      <c r="B38" t="s">
+    <row r="42" spans="1:7">
+      <c r="B42" t="s">
         <v>145</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C42" t="s">
         <v>146</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G42" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
-      <c r="B39" t="s">
+    <row r="43" spans="1:7">
+      <c r="B43" t="s">
         <v>150</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C43" t="s">
         <v>152</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G43" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
-      <c r="B40" t="s">
+    <row r="44" spans="1:7">
+      <c r="B44" t="s">
         <v>151</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C44" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
-      <c r="B41" t="s">
+    <row r="45" spans="1:7">
+      <c r="B45" t="s">
         <v>155</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C45" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2487,9 +2535,9 @@
     <hyperlink ref="Z5" r:id="rId1"/>
     <hyperlink ref="Z6" r:id="rId2"/>
     <hyperlink ref="Z7" r:id="rId3"/>
-    <hyperlink ref="A31" r:id="rId4"/>
-    <hyperlink ref="A29" r:id="rId5"/>
-    <hyperlink ref="A27" r:id="rId6"/>
+    <hyperlink ref="A35" r:id="rId4"/>
+    <hyperlink ref="A33" r:id="rId5"/>
+    <hyperlink ref="A31" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
restructured filetree, edit user bugged, delete user implemented
</commit_message>
<xml_diff>
--- a/assets/Project 2 Planning.xlsx
+++ b/assets/Project 2 Planning.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Functional Components" sheetId="2" r:id="rId2"/>
     <sheet name="Features" sheetId="3" r:id="rId3"/>
+    <sheet name="Table Flow Diagrams" sheetId="4" r:id="rId4"/>
+    <sheet name="Google Places" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,30 +23,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="166">
   <si>
     <t xml:space="preserve">Unit 2 Project </t>
-  </si>
-  <si>
-    <t xml:space="preserve">To Do's </t>
-  </si>
-  <si>
-    <t>In Progress</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
-    <t>Issues</t>
-  </si>
-  <si>
-    <t>Wireframe</t>
-  </si>
-  <si>
-    <t>Priority Matrix</t>
-  </si>
-  <si>
-    <t>Approval</t>
   </si>
   <si>
     <t>Day</t>
@@ -525,7 +506,22 @@
     <t>Create New Blog Entry</t>
   </si>
   <si>
-    <t>Clickable Model</t>
+    <t>Landing page: Login Button, Register New User, Public Directory of Users</t>
+  </si>
+  <si>
+    <t>Public Directory of Users: Gallery of usernames, links to Individual Public Profiles</t>
+  </si>
+  <si>
+    <t>Individual Public Profiles: Display user's username, email and avatar, sample list of blog entries links to individual public blog entry</t>
+  </si>
+  <si>
+    <t>Individual Public Blog Entry: Input text fields, Post button, Edit Button, Delete Button</t>
+  </si>
+  <si>
+    <t>User Authentication</t>
+  </si>
+  <si>
+    <t>Schedule</t>
   </si>
 </sst>
 </file>
@@ -858,16 +854,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -891,7 +887,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="15354300" y="6146800"/>
+          <a:off x="0" y="0"/>
           <a:ext cx="6032500" cy="7391400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -937,19 +933,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:E14" totalsRowShown="0">
-  <autoFilter ref="B3:E14"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="To Do's "/>
-    <tableColumn id="2" name="In Progress"/>
-    <tableColumn id="3" name="Completed"/>
-    <tableColumn id="4" name="Issues"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1274,23 +1257,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF45"/>
+  <dimension ref="A1:AF31"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17:F21"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
-    <col min="2" max="5" width="11" customWidth="1"/>
+    <col min="2" max="2" width="2.83203125" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="2.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="43" customWidth="1"/>
-    <col min="13" max="13" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="2.1640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="2.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1302,584 +1289,611 @@
     </row>
     <row r="3" spans="1:32">
       <c r="B3" t="s">
+        <v>165</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="W3" s="2"/>
+    </row>
+    <row r="4" spans="1:32">
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" t="s">
-        <v>9</v>
-      </c>
-      <c r="W3" s="2" t="s">
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="R4" s="2"/>
+    </row>
+    <row r="5" spans="1:32">
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="4" spans="1:32">
-      <c r="W4" t="s">
+      <c r="O5" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="X4" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y4" t="s">
+      <c r="P5" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="Z4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>74</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32">
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" t="s">
-        <v>49</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="W5">
-        <v>1</v>
-      </c>
-      <c r="X5" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z5" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>105</v>
-      </c>
+      <c r="Q5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="R5" s="2"/>
+      <c r="Z5" s="4"/>
       <c r="AF5" s="3"/>
     </row>
     <row r="6" spans="1:32">
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" t="s">
-        <v>50</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="W6">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="2">
         <v>2</v>
       </c>
-      <c r="X6" t="s">
-        <v>100</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>101</v>
-      </c>
-      <c r="Z6" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>104</v>
-      </c>
+      <c r="M6" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="R6" s="2"/>
+      <c r="Z6" s="4"/>
     </row>
     <row r="7" spans="1:32">
       <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="2">
+        <v>3</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="R7" s="2"/>
+      <c r="Z7" s="4"/>
+    </row>
+    <row r="8" spans="1:32">
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8" s="2">
+        <v>4</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+    </row>
+    <row r="9" spans="1:32">
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9" s="2">
+        <v>5</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+    </row>
+    <row r="10" spans="1:32">
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
         <v>7</v>
       </c>
-      <c r="F7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="W7">
-        <v>3</v>
-      </c>
-      <c r="X7" t="s">
-        <v>106</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>107</v>
-      </c>
-      <c r="Z7" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>109</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32">
-      <c r="F8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+    </row>
+    <row r="11" spans="1:32">
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
         <v>13</v>
       </c>
-      <c r="H8" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="W8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32">
-      <c r="F9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="W9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32">
-      <c r="F10" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" t="s">
-        <v>45</v>
-      </c>
-      <c r="I10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:32">
-      <c r="F11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" t="s">
-        <v>45</v>
-      </c>
-      <c r="I11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="W11" t="s">
-        <v>79</v>
-      </c>
+      <c r="F11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
     </row>
     <row r="12" spans="1:32">
-      <c r="W12" t="s">
-        <v>70</v>
-      </c>
-      <c r="X12" t="s">
-        <v>80</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>82</v>
-      </c>
-      <c r="AA12" t="s">
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+    </row>
+    <row r="13" spans="1:32">
+      <c r="L13" s="2">
+        <v>1</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="O13" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="13" spans="1:32">
-      <c r="W13">
+      <c r="P13" s="2">
         <v>1</v>
       </c>
-      <c r="X13" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y13" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>90</v>
-      </c>
-      <c r="AA13">
-        <v>1</v>
-      </c>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="Y13" s="3"/>
     </row>
     <row r="14" spans="1:32">
+      <c r="A14" t="s">
+        <v>151</v>
+      </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="W14">
+      <c r="L14" s="2">
         <v>2</v>
       </c>
-      <c r="X14" t="s">
+      <c r="M14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="P14" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+    </row>
+    <row r="15" spans="1:32">
+      <c r="A15" t="s">
+        <v>150</v>
+      </c>
+      <c r="L15" s="2">
+        <v>3</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="P15" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+    </row>
+    <row r="16" spans="1:32">
+      <c r="L16" s="2">
+        <v>4</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O16" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="Y14" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>91</v>
-      </c>
-      <c r="AA14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32">
-      <c r="W15">
-        <v>3</v>
-      </c>
-      <c r="X15" t="s">
+      <c r="P16" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+    </row>
+    <row r="17" spans="1:21">
+      <c r="A17" t="s">
+        <v>144</v>
+      </c>
+      <c r="L17" s="2">
+        <v>5</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="O17" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="Y15" t="s">
-        <v>97</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:32">
-      <c r="W16">
-        <v>4</v>
-      </c>
-      <c r="X16" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>93</v>
-      </c>
-      <c r="AA16">
+      <c r="P17" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:28">
-      <c r="W17">
-        <v>5</v>
-      </c>
-      <c r="X17" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28">
-      <c r="W20" t="s">
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+    </row>
+    <row r="18" spans="1:21">
+      <c r="A18" t="s">
+        <v>145</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+    </row>
+    <row r="19" spans="1:21">
+      <c r="A19" t="s">
+        <v>146</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+    </row>
+    <row r="20" spans="1:21">
+      <c r="A20" t="s">
+        <v>147</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="R20" s="2"/>
+    </row>
+    <row r="21" spans="1:21">
+      <c r="L21" s="2"/>
+      <c r="M21" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="R21" s="2"/>
+    </row>
+    <row r="22" spans="1:21">
+      <c r="L22" s="2"/>
+      <c r="M22" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="R22" s="2"/>
+    </row>
+    <row r="23" spans="1:21">
+      <c r="L23" s="2"/>
+      <c r="M23" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="X20" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y20" t="s">
+      <c r="Q23" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="R23" s="2"/>
+    </row>
+    <row r="24" spans="1:21">
+      <c r="L24" s="2"/>
+      <c r="M24" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="AA20" t="s">
-        <v>123</v>
-      </c>
-      <c r="AB20" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28">
-      <c r="X21" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA21" t="s">
-        <v>112</v>
-      </c>
-      <c r="AB21" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28">
-      <c r="X22" t="s">
-        <v>113</v>
-      </c>
-      <c r="Y22" t="s">
+      <c r="Q24" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="R24" s="2"/>
+    </row>
+    <row r="25" spans="1:21">
+      <c r="L25" s="2"/>
+      <c r="M25" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q25" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="AA22" t="s">
-        <v>124</v>
-      </c>
-      <c r="AB22" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="23" spans="1:28">
-      <c r="X23" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>121</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>125</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28">
-      <c r="X24" t="s">
+      <c r="R25" s="2"/>
+    </row>
+    <row r="26" spans="1:21">
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+    </row>
+    <row r="30" spans="1:21">
+      <c r="L30" s="2"/>
+      <c r="M30" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="N30" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="Y24" t="s">
-        <v>121</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>126</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28">
-      <c r="X25" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>121</v>
-      </c>
-      <c r="AA25" t="s">
-        <v>83</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28">
-      <c r="G27" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28">
-      <c r="A28" t="s">
-        <v>156</v>
-      </c>
-      <c r="G28" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28">
-      <c r="A29" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="30" spans="1:28">
-      <c r="A30" t="s">
-        <v>132</v>
-      </c>
-      <c r="X30" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y30" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="31" spans="1:28">
-      <c r="A31" s="4" t="s">
-        <v>133</v>
-      </c>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
       <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
       <c r="S31" s="2"/>
       <c r="U31" s="2"/>
     </row>
-    <row r="32" spans="1:28">
-      <c r="A32" t="s">
-        <v>129</v>
-      </c>
-      <c r="T32" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="60">
-      <c r="A40" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G40" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B41" t="s">
-        <v>139</v>
-      </c>
-      <c r="C41" t="s">
-        <v>137</v>
-      </c>
-      <c r="G41" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="B42" t="s">
-        <v>140</v>
-      </c>
-      <c r="C42" t="s">
-        <v>141</v>
-      </c>
-      <c r="G42" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="B43" t="s">
-        <v>145</v>
-      </c>
-      <c r="C43" t="s">
-        <v>147</v>
-      </c>
-      <c r="G43" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="B44" t="s">
-        <v>146</v>
-      </c>
-      <c r="C44" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="B45" t="s">
-        <v>150</v>
-      </c>
-      <c r="C45" t="s">
-        <v>149</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Z5" r:id="rId1"/>
-    <hyperlink ref="Z6" r:id="rId2"/>
-    <hyperlink ref="Z7" r:id="rId3"/>
-    <hyperlink ref="A35" r:id="rId4"/>
-    <hyperlink ref="A33" r:id="rId5"/>
-    <hyperlink ref="A31" r:id="rId6"/>
+    <hyperlink ref="O5" r:id="rId1"/>
+    <hyperlink ref="O6" r:id="rId2"/>
+    <hyperlink ref="O7" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId7"/>
-  <tableParts count="1">
-    <tablePart r:id="rId8"/>
-  </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1913,855 +1927,855 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="B1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
         <v>45</v>
       </c>
-      <c r="D3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
         <v>45</v>
       </c>
-      <c r="F3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" t="s">
         <v>45</v>
       </c>
-      <c r="H3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I3" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" t="s">
-        <v>52</v>
-      </c>
       <c r="K3" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J4">
         <v>0.2</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F5">
         <v>0.5</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H5">
         <v>0.5</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J5">
         <v>0.5</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F6">
         <v>0.5</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" t="s">
-        <v>38</v>
-      </c>
       <c r="E7" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J7">
         <v>3</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J8">
         <v>1</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F9">
         <v>1.5</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J9">
         <v>1</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F11">
         <v>0.5</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F12">
         <v>2</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F13">
         <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F15">
         <v>2</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F16">
         <v>0.5</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F17">
         <v>2</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F18">
         <v>2</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F19">
         <v>0.5</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E22" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F22">
         <v>0.5</v>
       </c>
       <c r="G22" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I22" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K22" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E23" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F23">
         <v>1.5</v>
       </c>
       <c r="G23" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I23" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K23" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F24">
         <v>1.5</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D25" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F25">
         <v>1.5</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E27" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I27" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K27" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E28" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G28" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I28" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K28" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F29">
         <f>SUM(F4:F27)</f>
         <v>30</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H29">
         <f>SUM(H4:H27)</f>
         <v>3.5</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J29">
         <f>SUM(J4:J27)</f>
         <v>5.7</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2777,125 +2791,204 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="48.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="B1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
         <v>53</v>
       </c>
-      <c r="F1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="C3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="C4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="C5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="C6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" t="s">
-        <v>60</v>
+      <c r="E6" t="s">
+        <v>47</v>
       </c>
       <c r="F6" t="s">
         <v>54</v>
       </c>
       <c r="G6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>47</v>
+      </c>
+      <c r="H6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="C7" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="C8" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="C9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" t="s">
-        <v>57</v>
+        <v>52</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2907,4 +3000,152 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C19"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14:G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="60">
+      <c r="A14" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" t="s">
+        <v>139</v>
+      </c>
+      <c r="C18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" t="s">
+        <v>143</v>
+      </c>
+      <c r="C19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A9" r:id="rId1"/>
+    <hyperlink ref="A7" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
light design enhancements to directory
</commit_message>
<xml_diff>
--- a/assets/Project 2 Planning.xlsx
+++ b/assets/Project 2 Planning.xlsx
@@ -4,15 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="0" windowWidth="21460" windowHeight="15460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="4140" yWindow="0" windowWidth="21460" windowHeight="15460" tabRatio="500" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Filetree" sheetId="6" r:id="rId2"/>
-    <sheet name="Functional Components" sheetId="2" r:id="rId3"/>
-    <sheet name="Features" sheetId="3" r:id="rId4"/>
-    <sheet name="Table Flow Diagrams" sheetId="4" r:id="rId5"/>
-    <sheet name="Google Places" sheetId="5" r:id="rId6"/>
+    <sheet name="Main" sheetId="1" r:id="rId1"/>
+    <sheet name="Errors" sheetId="7" r:id="rId2"/>
+    <sheet name="Filetree" sheetId="6" r:id="rId3"/>
+    <sheet name="Functional Components" sheetId="2" r:id="rId4"/>
+    <sheet name="Features" sheetId="3" r:id="rId5"/>
+    <sheet name="Table Flow Diagrams" sheetId="4" r:id="rId6"/>
+    <sheet name="Google Places" sheetId="5" r:id="rId7"/>
+    <sheet name="Schedule" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="218">
   <si>
     <t xml:space="preserve">Unit 2 Project </t>
   </si>
@@ -630,9 +633,6 @@
     <t>Problem with action="" missing / at beginning</t>
   </si>
   <si>
-    <t>3:1 Refused to apply style from 'http://localhost:3000/public/css/style.css' because its MIME type ('text/html') is not a supported stylesheet MIME type, and strict MIME checking is enabled.</t>
-  </si>
-  <si>
     <t>https://github.com/RonAddy/Sample_Express_App_Auth</t>
   </si>
   <si>
@@ -652,6 +652,36 @@
   </si>
   <si>
     <t>Authorization - Public - Private Page Access - Implementation</t>
+  </si>
+  <si>
+    <t>Refused to apply style from 'http://localhost:3000/public/css/style.css' because its MIME type ('text/html') is not a supported stylesheet MIME type, and strict MIME checking is enabled.</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>Sources</t>
+  </si>
+  <si>
+    <t>Question mark png</t>
+  </si>
+  <si>
+    <t>http://pngimg.com/uploads/question_mark/question_mark_PNG129.png</t>
+  </si>
+  <si>
+    <t>Thing</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>Sessions-Authentication Tutorial</t>
   </si>
 </sst>
 </file>
@@ -1387,670 +1417,506 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ32"/>
+  <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView showRuler="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="2.83203125" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
-      <c r="B3" t="s">
-        <v>164</v>
-      </c>
-      <c r="H3" t="s">
-        <v>196</v>
-      </c>
-      <c r="L3" t="s">
+    <row r="3" spans="1:27">
+      <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" t="s">
         <v>165</v>
       </c>
-      <c r="V3" s="2"/>
-      <c r="AA3" s="2"/>
-    </row>
-    <row r="4" spans="1:36">
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="M3" s="2"/>
+      <c r="R3" s="2"/>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="A4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:27">
+      <c r="C5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="U5" s="4"/>
+      <c r="AA5" s="3"/>
+    </row>
+    <row r="6" spans="1:27">
+      <c r="A6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="2">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="U6" s="4"/>
+    </row>
+    <row r="7" spans="1:27">
+      <c r="A7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="2">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="V4" s="2"/>
-    </row>
-    <row r="5" spans="1:36">
-      <c r="B5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" t="s">
-        <v>197</v>
-      </c>
-      <c r="I5" t="s">
-        <v>198</v>
-      </c>
-      <c r="L5" s="2" t="s">
+      <c r="D7" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="U7" s="4"/>
+    </row>
+    <row r="8" spans="1:27">
+      <c r="A8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:27">
+      <c r="A9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:27">
+      <c r="C10" s="2">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:27">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:27">
+      <c r="A12" t="s">
+        <v>201</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:27">
+      <c r="C13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="V5" s="2"/>
-      <c r="AD5" s="4"/>
-      <c r="AJ5" s="3"/>
-    </row>
-    <row r="6" spans="1:36">
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="T13" s="3"/>
+    </row>
+    <row r="14" spans="1:27">
+      <c r="B14" s="1"/>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:27">
+      <c r="C15" s="2">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:27">
+      <c r="C16" s="2">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" t="s">
-        <v>199</v>
-      </c>
-      <c r="I6" t="s">
-        <v>200</v>
-      </c>
-      <c r="L6" s="2">
+      <c r="D16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="2">
         <v>1</v>
       </c>
-      <c r="M6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="V6" s="2"/>
-      <c r="AD6" s="4"/>
-    </row>
-    <row r="7" spans="1:36">
-      <c r="B7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="H16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="3:16">
+      <c r="C17" s="2">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" t="s">
-        <v>201</v>
-      </c>
-      <c r="L7" s="2">
+      <c r="D17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" s="2">
         <v>2</v>
       </c>
-      <c r="M7" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="V7" s="2"/>
-      <c r="AD7" s="4"/>
-    </row>
-    <row r="8" spans="1:36">
-      <c r="B8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="H17" s="2"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="3:16">
+      <c r="C18" s="2">
         <v>5</v>
       </c>
-      <c r="D8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L8" s="2">
-        <v>3</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="V8" s="2"/>
-    </row>
-    <row r="9" spans="1:36">
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L9" s="2">
-        <v>4</v>
-      </c>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="V9" s="2"/>
-    </row>
-    <row r="10" spans="1:36">
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L10" s="2">
-        <v>5</v>
-      </c>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="V10" s="2"/>
-    </row>
-    <row r="11" spans="1:36">
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="V11" s="2"/>
-    </row>
-    <row r="12" spans="1:36">
-      <c r="B12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="V12" s="2"/>
-    </row>
-    <row r="13" spans="1:36">
-      <c r="L13" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="P13" s="2" t="s">
+      <c r="D18" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="2">
+        <v>2</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="3:16">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="3:16">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="3:16">
+      <c r="C21" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="3:16">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="3:16">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="3:16">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="3:16">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="M25" s="2"/>
+    </row>
+    <row r="26" spans="3:16">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="Q13" s="2"/>
-      <c r="V13" s="2"/>
-      <c r="AC13" s="3"/>
-    </row>
-    <row r="14" spans="1:36">
-      <c r="A14" t="s">
-        <v>150</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="L14" s="2">
-        <v>1</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="P14" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="2"/>
-      <c r="V14" s="2"/>
-    </row>
-    <row r="15" spans="1:36">
-      <c r="A15" t="s">
-        <v>149</v>
-      </c>
-      <c r="L15" s="2">
-        <v>2</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="P15" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="2"/>
-      <c r="V15" s="2"/>
-    </row>
-    <row r="16" spans="1:36">
-      <c r="L16" s="2">
-        <v>3</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="P16" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="2"/>
-      <c r="V16" s="2"/>
-    </row>
-    <row r="17" spans="1:25">
-      <c r="A17" t="s">
-        <v>143</v>
-      </c>
-      <c r="L17" s="2">
-        <v>4</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="P17" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q17" s="2"/>
-      <c r="V17" s="2"/>
-    </row>
-    <row r="18" spans="1:25">
-      <c r="A18" t="s">
-        <v>144</v>
-      </c>
-      <c r="L18" s="2">
-        <v>5</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="P18" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q18" s="2"/>
-      <c r="V18" s="2"/>
-    </row>
-    <row r="19" spans="1:25">
-      <c r="A19" t="s">
-        <v>145</v>
-      </c>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="V19" s="2"/>
-    </row>
-    <row r="20" spans="1:25">
-      <c r="A20" t="s">
-        <v>146</v>
-      </c>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="V20" s="2"/>
-    </row>
-    <row r="21" spans="1:25">
-      <c r="L21" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q21" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="V21" s="2"/>
-    </row>
-    <row r="22" spans="1:25">
-      <c r="A22" t="s">
-        <v>19</v>
-      </c>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="V22" s="2"/>
-    </row>
-    <row r="23" spans="1:25">
-      <c r="A23" t="s">
-        <v>202</v>
-      </c>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="N23" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q23" s="2" t="s">
+      <c r="H26" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="3:16">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="M27" s="2"/>
+    </row>
+    <row r="28" spans="3:16">
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="M28" s="2"/>
+    </row>
+    <row r="29" spans="3:16">
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="M29" s="2"/>
+    </row>
+    <row r="30" spans="3:16">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="M30" s="2"/>
+    </row>
+    <row r="31" spans="3:16">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="V23" s="2"/>
-    </row>
-    <row r="24" spans="1:25">
-      <c r="L24" s="2"/>
-      <c r="M24" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="N24" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q24" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="V24" s="2"/>
-    </row>
-    <row r="25" spans="1:25">
-      <c r="L25" s="2"/>
-      <c r="M25" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="N25" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q25" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="V25" s="2"/>
-    </row>
-    <row r="26" spans="1:25">
-      <c r="L26" s="2"/>
-      <c r="M26" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="N26" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q26" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="V26" s="2"/>
-    </row>
-    <row r="27" spans="1:25">
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
-      <c r="V27" s="2"/>
-    </row>
-    <row r="28" spans="1:25">
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
-      <c r="V28" s="2"/>
-    </row>
-    <row r="29" spans="1:25">
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
-      <c r="V29" s="2"/>
-    </row>
-    <row r="30" spans="1:25">
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-      <c r="Q30" s="2"/>
-      <c r="V30" s="2"/>
-    </row>
-    <row r="31" spans="1:25">
-      <c r="L31" s="2"/>
-      <c r="M31" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="N31" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="O31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
       <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="V31" s="2"/>
-      <c r="W31" s="2"/>
-      <c r="Y31" s="2"/>
-    </row>
-    <row r="32" spans="1:25">
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-      <c r="Q32" s="2"/>
+    </row>
+    <row r="32" spans="3:16">
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O6" r:id="rId1"/>
-    <hyperlink ref="O7" r:id="rId2"/>
-    <hyperlink ref="O8" r:id="rId3"/>
+    <hyperlink ref="F6" r:id="rId1"/>
+    <hyperlink ref="F7" r:id="rId2"/>
+    <hyperlink ref="F8" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2064,6 +1930,67 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="47.83203125" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="A2" workbookViewId="0">
@@ -2264,12 +2191,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2782,8 +2709,11 @@
       </c>
     </row>
     <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
       <c r="B17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C17" t="s">
         <v>39</v>
@@ -2812,7 +2742,7 @@
         <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C18" t="s">
         <v>39</v>
@@ -2837,8 +2767,11 @@
       </c>
     </row>
     <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
       <c r="B19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C19" t="s">
         <v>39</v>
@@ -2863,8 +2796,11 @@
       </c>
     </row>
     <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
       <c r="B20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C20" t="s">
         <v>39</v>
@@ -2889,8 +2825,11 @@
       </c>
     </row>
     <row r="21" spans="1:11">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
       <c r="B21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C21" t="s">
         <v>39</v>
@@ -2919,7 +2858,7 @@
         <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C22" t="s">
         <v>39</v>
@@ -3270,7 +3209,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -3483,7 +3422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3501,7 +3440,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C19"/>
   <sheetViews>
@@ -3629,4 +3568,234 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
return json of all blog entries
</commit_message>
<xml_diff>
--- a/assets/Project 2 Planning.xlsx
+++ b/assets/Project 2 Planning.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Table Flow Diagrams" sheetId="4" r:id="rId6"/>
     <sheet name="Google Places" sheetId="5" r:id="rId7"/>
     <sheet name="Schedule" sheetId="8" r:id="rId8"/>
-    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
+    <sheet name="Add Sources" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="222">
   <si>
     <t xml:space="preserve">Unit 2 Project </t>
   </si>
@@ -682,6 +682,18 @@
   </si>
   <si>
     <t>Sessions-Authentication Tutorial</t>
+  </si>
+  <si>
+    <t>date_created</t>
+  </si>
+  <si>
+    <t>Convert CSV</t>
+  </si>
+  <si>
+    <t>http://www.convertcsv.com/</t>
+  </si>
+  <si>
+    <t>random gen data</t>
   </si>
 </sst>
 </file>
@@ -1419,8 +1431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView showRuler="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1846,11 +1858,9 @@
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>120</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="H26" s="2"/>
       <c r="M26" s="2"/>
     </row>
     <row r="27" spans="3:16">
@@ -1858,8 +1868,12 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
+      <c r="G27" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="M27" s="2"/>
     </row>
     <row r="28" spans="3:16">
@@ -1867,8 +1881,6 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
       <c r="M28" s="2"/>
     </row>
     <row r="29" spans="3:16">
@@ -3750,10 +3762,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3761,12 +3773,12 @@
     <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>215</v>
       </c>
@@ -3774,7 +3786,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>213</v>
       </c>
@@ -3782,12 +3794,23 @@
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>217</v>
       </c>
       <c r="B4" t="s">
         <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C5" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
return json of single blog post
</commit_message>
<xml_diff>
--- a/assets/Project 2 Planning.xlsx
+++ b/assets/Project 2 Planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="0" windowWidth="21460" windowHeight="15460" tabRatio="500" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="4140" yWindow="-20" windowWidth="21460" windowHeight="15520" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Schedule" sheetId="8" r:id="rId8"/>
     <sheet name="Add Sources" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="224">
   <si>
     <t xml:space="preserve">Unit 2 Project </t>
   </si>
@@ -694,6 +694,12 @@
   </si>
   <si>
     <t>random gen data</t>
+  </si>
+  <si>
+    <t>SyntaxError: Unexpected token {</t>
+  </si>
+  <si>
+    <t>extra } after object function</t>
   </si>
 </sst>
 </file>
@@ -1931,7 +1937,6 @@
     <hyperlink ref="F8" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1942,10 +1947,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1989,6 +1994,14 @@
       </c>
       <c r="B5" t="s">
         <v>209</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B6" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -2194,7 +2207,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3212,7 +3224,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3425,7 +3436,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3573,7 +3583,6 @@
     <hyperlink ref="A5" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3764,8 +3773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
rendered private user profile page
</commit_message>
<xml_diff>
--- a/assets/Project 2 Planning.xlsx
+++ b/assets/Project 2 Planning.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="225">
   <si>
     <t xml:space="preserve">Unit 2 Project </t>
   </si>
@@ -700,6 +700,9 @@
   </si>
   <si>
     <t>extra } after object function</t>
+  </si>
+  <si>
+    <t>Error [ERR_HTTP_HEADERS_SENT]: Cannot set headers after they are sent to the client</t>
   </si>
 </sst>
 </file>
@@ -1947,10 +1950,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2002,6 +2005,11 @@
       </c>
       <c r="B6" t="s">
         <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rendered private user profile view with links connecting to rendered private user blog entry view
</commit_message>
<xml_diff>
--- a/assets/Project 2 Planning.xlsx
+++ b/assets/Project 2 Planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="-20" windowWidth="21460" windowHeight="15520" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="230">
   <si>
     <t xml:space="preserve">Unit 2 Project </t>
   </si>
@@ -703,6 +703,21 @@
   </si>
   <si>
     <t>Error [ERR_HTTP_HEADERS_SENT]: Cannot set headers after they are sent to the client</t>
+  </si>
+  <si>
+    <t>Multiple responses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">error: invalid input syntax for integer: "Do ic zetawde ba eboztog </t>
+  </si>
+  <si>
+    <t>Route.get() requires a callback function but got a [object Undefined]</t>
+  </si>
+  <si>
+    <t>Incorrect call in route to nonexistent function</t>
+  </si>
+  <si>
+    <t>Trying to return data in improper format</t>
   </si>
 </sst>
 </file>
@@ -1950,10 +1965,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2010,6 +2025,25 @@
     <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>224</v>
+      </c>
+      <c r="B7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>227</v>
+      </c>
+      <c r="B9" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create new blog entry is functional
</commit_message>
<xml_diff>
--- a/assets/Project 2 Planning.xlsx
+++ b/assets/Project 2 Planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="15600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="240">
   <si>
     <t xml:space="preserve">Unit 2 Project </t>
   </si>
@@ -718,13 +718,43 @@
   </si>
   <si>
     <t>Trying to return data in improper format</t>
+  </si>
+  <si>
+    <t>Cannot POST /private/entries/</t>
+  </si>
+  <si>
+    <t>Cannot POST /private/users/[object%20Object],[object%20Object],[object%20Object],[object%20Object],[object%20Object]</t>
+  </si>
+  <si>
+    <t>error: syntax error at or near "$"</t>
+  </si>
+  <si>
+    <t>mistake in createNewEntry params, fixed to req, res, next</t>
+  </si>
+  <si>
+    <t>Error: Property 'date_created' doesn't exist.</t>
+  </si>
+  <si>
+    <t>mistake in createNewEntry params, fixed to req.body</t>
+  </si>
+  <si>
+    <t>Needed to specify a real date</t>
+  </si>
+  <si>
+    <t>I am error:  { error: date/time field value out of range: "123123123", I am error:  { error: invalid input syntax for type date: "reeqwr"</t>
+  </si>
+  <si>
+    <t>I am error:  Error: Property 'user_id' doesn't exist.</t>
+  </si>
+  <si>
+    <t>Needed to specify user_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -768,6 +798,11 @@
       <color rgb="FF505050"/>
       <name val="Helvetica"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -907,7 +942,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -919,6 +954,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="119">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1456,7 +1492,7 @@
   <dimension ref="A1:AA32"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26:H27"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1965,10 +2001,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2044,6 +2080,48 @@
       </c>
       <c r="B9" t="s">
         <v>228</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="B12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>237</v>
+      </c>
+      <c r="B14" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B15" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update blog entry functional
</commit_message>
<xml_diff>
--- a/assets/Project 2 Planning.xlsx
+++ b/assets/Project 2 Planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="15600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="27880" yWindow="-940" windowWidth="25600" windowHeight="15600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="242">
   <si>
     <t xml:space="preserve">Unit 2 Project </t>
   </si>
@@ -748,6 +748,12 @@
   </si>
   <si>
     <t>Needed to specify user_id</t>
+  </si>
+  <si>
+    <t>error: time zone "gmt-0400" not recognized</t>
+  </si>
+  <si>
+    <t>Table Schema Issue, removing Date spec</t>
   </si>
 </sst>
 </file>
@@ -2001,10 +2007,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2122,6 +2128,14 @@
       </c>
       <c r="B15" t="s">
         <v>239</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="B16" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
boilerplate setup for user public profile views, non-functional
</commit_message>
<xml_diff>
--- a/assets/Project 2 Planning.xlsx
+++ b/assets/Project 2 Planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="27880" yWindow="-940" windowWidth="25600" windowHeight="15600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="244">
   <si>
     <t xml:space="preserve">Unit 2 Project </t>
   </si>
@@ -754,6 +754,12 @@
   </si>
   <si>
     <t>Set Absolute path to css i.e. /../css/style.css instead of ../css/style.css</t>
+  </si>
+  <si>
+    <t>PSQL Queries</t>
+  </si>
+  <si>
+    <t>SELECT * FROM users JOIN blog_entries ON users.id = blog_entries.user_id;</t>
   </si>
 </sst>
 </file>
@@ -1497,8 +1503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1543,6 +1549,9 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
+      <c r="J4" t="s">
+        <v>242</v>
+      </c>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:27">
@@ -1563,6 +1572,9 @@
       </c>
       <c r="H5" s="2" t="s">
         <v>76</v>
+      </c>
+      <c r="J5" t="s">
+        <v>243</v>
       </c>
       <c r="M5" s="2"/>
       <c r="U5" s="4"/>
@@ -2009,7 +2021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView showRuler="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
have working authentication, needs debugging if user entries = 0
</commit_message>
<xml_diff>
--- a/assets/Project 2 Planning.xlsx
+++ b/assets/Project 2 Planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="255">
   <si>
     <t xml:space="preserve">Unit 2 Project </t>
   </si>
@@ -760,6 +760,41 @@
   </si>
   <si>
     <t>SELECT * FROM users JOIN blog_entries ON users.id = blog_entries.user_id;</t>
+  </si>
+  <si>
+    <t>* Express</t>
+  </si>
+  <si>
+    <t>* Pg Promise</t>
+  </si>
+  <si>
+    <t>* bodyParser</t>
+  </si>
+  <si>
+    <t>* Nodemon</t>
+  </si>
+  <si>
+    <t>* Morgan</t>
+  </si>
+  <si>
+    <t>* Dotenv</t>
+  </si>
+  <si>
+    <t>* Express Session</t>
+  </si>
+  <si>
+    <t>* Method Override</t>
+  </si>
+  <si>
+    <t>* Faker</t>
+  </si>
+  <si>
+    <t>Additional Libraries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"error": {
+"name": "QueryResultError",
+"stack": "QueryResultError: 0\n    at new QueryResultError </t>
   </si>
 </sst>
 </file>
@@ -1503,8 +1538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA32"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView showRuler="0" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1553,6 +1588,9 @@
         <v>242</v>
       </c>
       <c r="M4" s="2"/>
+      <c r="O4" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="5" spans="1:27">
       <c r="C5" s="2" t="s">
@@ -1577,6 +1615,9 @@
         <v>243</v>
       </c>
       <c r="M5" s="2"/>
+      <c r="N5" t="s">
+        <v>244</v>
+      </c>
       <c r="U5" s="4"/>
       <c r="AA5" s="3"/>
     </row>
@@ -1603,6 +1644,9 @@
         <v>97</v>
       </c>
       <c r="M6" s="2"/>
+      <c r="N6" t="s">
+        <v>245</v>
+      </c>
       <c r="U6" s="4"/>
     </row>
     <row r="7" spans="1:27">
@@ -1628,6 +1672,9 @@
         <v>96</v>
       </c>
       <c r="M7" s="2"/>
+      <c r="N7" t="s">
+        <v>246</v>
+      </c>
       <c r="U7" s="4"/>
     </row>
     <row r="8" spans="1:27">
@@ -1653,6 +1700,9 @@
         <v>102</v>
       </c>
       <c r="M8" s="2"/>
+      <c r="N8" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="9" spans="1:27">
       <c r="A9" t="s">
@@ -1667,6 +1717,9 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="M9" s="2"/>
+      <c r="N9" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="10" spans="1:27">
       <c r="C10" s="2">
@@ -1678,6 +1731,9 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="M10" s="2"/>
+      <c r="N10" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="11" spans="1:27">
       <c r="A11" t="s">
@@ -1690,6 +1746,9 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="M11" s="2"/>
+      <c r="N11" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="12" spans="1:27">
       <c r="A12" t="s">
@@ -1704,6 +1763,9 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="M12" s="2"/>
+      <c r="N12" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="13" spans="1:27">
       <c r="C13" s="2" t="s">
@@ -1723,6 +1785,9 @@
       </c>
       <c r="H13" s="2"/>
       <c r="M13" s="2"/>
+      <c r="N13" t="s">
+        <v>252</v>
+      </c>
       <c r="T13" s="3"/>
     </row>
     <row r="14" spans="1:27">
@@ -1819,6 +1884,9 @@
         <v>2</v>
       </c>
       <c r="H18" s="2"/>
+      <c r="J18" t="s">
+        <v>68</v>
+      </c>
       <c r="M18" s="2"/>
     </row>
     <row r="19" spans="3:16">
@@ -2019,10 +2087,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2148,6 +2216,11 @@
       </c>
       <c r="B16" t="s">
         <v>240</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="60">
+      <c r="A17" s="6" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Debugged one public user profile view, one public user blog entry view
</commit_message>
<xml_diff>
--- a/assets/Project 2 Planning.xlsx
+++ b/assets/Project 2 Planning.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="261">
   <si>
     <t xml:space="preserve">Unit 2 Project </t>
   </si>
@@ -795,6 +795,27 @@
     <t xml:space="preserve">"error": {
 "name": "QueryResultError",
 "stack": "QueryResultError: 0\n    at new QueryResultError </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  showHomepage(req, res) {
+  ^^^^^^^^^^^^
+SyntaxError: Unexpected identifier</t>
+  </si>
+  <si>
+    <t>module.exports object missing , after }</t>
+  </si>
+  <si>
+    <t>WYSIWYG Editor</t>
+  </si>
+  <si>
+    <t>https://yuilibrary.com/</t>
+  </si>
+  <si>
+    <t>"error": {},
+"message": "publicDb is not defined"</t>
+  </si>
+  <si>
+    <t>Syntax Error, "publicDB"</t>
   </si>
 </sst>
 </file>
@@ -1536,10 +1557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA32"/>
+  <dimension ref="A1:AA34"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView showRuler="0" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2070,6 +2091,16 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>258</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1"/>
@@ -2087,10 +2118,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2218,9 +2249,25 @@
         <v>240</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="60">
+    <row r="17" spans="1:2" ht="60">
       <c r="A17" s="6" t="s">
         <v>254</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="60">
+      <c r="A18" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="B18" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="30">
+      <c r="A19" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="B19" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Debugged No Blog Entries, No User Profile View bug
</commit_message>
<xml_diff>
--- a/assets/Project 2 Planning.xlsx
+++ b/assets/Project 2 Planning.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="262">
   <si>
     <t xml:space="preserve">Unit 2 Project </t>
   </si>
@@ -816,6 +816,21 @@
   </si>
   <si>
     <t>Syntax Error, "publicDB"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am error:  QueryResultError {
+    code: queryResultErrorCode.noData
+    message: "No data returned from the query."
+    received: 0
+    query: "
+      SELECT *, blog_entries.id as entry_id
+        FROM users
+        JOIN blog_entries
+          ON users.id = blog_entries.user_id
+       WHERE users.id = '22'
+    "
+}
+</t>
   </si>
 </sst>
 </file>
@@ -2118,10 +2133,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2268,6 +2283,11 @@
       </c>
       <c r="B19" t="s">
         <v>260</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="195">
+      <c r="A20" s="6" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated project planning spreadsheet
</commit_message>
<xml_diff>
--- a/assets/Project 2 Planning.xlsx
+++ b/assets/Project 2 Planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="-16500" windowWidth="25600" windowHeight="14480" tabRatio="500" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -921,7 +921,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="122">
+  <cellStyleXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1022,6 +1022,85 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1060,7 +1139,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="122">
+  <cellStyles count="201">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1132,6 +1211,85 @@
     <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2161,7 +2319,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2317,6 +2475,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2530,7 +2689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:K33"/>
     </sheetView>
   </sheetViews>
@@ -2716,8 +2875,14 @@
       <c r="G6" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="H6">
+        <v>0.5</v>
+      </c>
       <c r="I6" s="2" t="s">
         <v>39</v>
+      </c>
+      <c r="J6">
+        <v>0.3</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>39</v>
@@ -2920,8 +3085,14 @@
       <c r="G12" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
       <c r="I12" s="2" t="s">
         <v>39</v>
+      </c>
+      <c r="J12">
+        <v>3</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>39</v>
@@ -2949,8 +3120,14 @@
       <c r="G13" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
       <c r="I13" s="2" t="s">
         <v>39</v>
+      </c>
+      <c r="J13">
+        <v>0.8</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>39</v>
@@ -2978,8 +3155,14 @@
       <c r="G14" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
       <c r="I14" s="2" t="s">
         <v>39</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>39</v>
@@ -3007,8 +3190,14 @@
       <c r="G15" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
       <c r="I15" s="2" t="s">
         <v>39</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>39</v>
@@ -3036,8 +3225,14 @@
       <c r="G16" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="H16">
+        <v>0.5</v>
+      </c>
       <c r="I16" s="2" t="s">
         <v>39</v>
+      </c>
+      <c r="J16">
+        <v>0.5</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>39</v>
@@ -3065,8 +3260,14 @@
       <c r="G17" t="s">
         <v>39</v>
       </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
       <c r="I17" t="s">
         <v>39</v>
+      </c>
+      <c r="J17">
+        <v>1.5</v>
       </c>
       <c r="K17" t="s">
         <v>39</v>
@@ -3094,8 +3295,14 @@
       <c r="G18" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="H18">
+        <v>0.5</v>
+      </c>
       <c r="I18" t="s">
         <v>39</v>
+      </c>
+      <c r="J18">
+        <v>0.5</v>
       </c>
       <c r="K18" t="s">
         <v>39</v>
@@ -3123,8 +3330,14 @@
       <c r="G19" t="s">
         <v>39</v>
       </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
       <c r="I19" t="s">
         <v>39</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
       </c>
       <c r="K19" t="s">
         <v>39</v>
@@ -3152,8 +3365,14 @@
       <c r="G20" t="s">
         <v>39</v>
       </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
       <c r="I20" t="s">
         <v>39</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
       </c>
       <c r="K20" t="s">
         <v>39</v>
@@ -3181,8 +3400,14 @@
       <c r="G21" t="s">
         <v>39</v>
       </c>
+      <c r="H21">
+        <v>0.5</v>
+      </c>
       <c r="I21" t="s">
         <v>39</v>
+      </c>
+      <c r="J21">
+        <v>0.7</v>
       </c>
       <c r="K21" t="s">
         <v>39</v>
@@ -3210,8 +3435,14 @@
       <c r="G22" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
       <c r="I22" s="2" t="s">
         <v>39</v>
+      </c>
+      <c r="J22">
+        <v>2</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>39</v>
@@ -3239,8 +3470,14 @@
       <c r="G23" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="H23">
+        <v>0.5</v>
+      </c>
       <c r="I23" s="2" t="s">
         <v>39</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>39</v>
@@ -3268,8 +3505,14 @@
       <c r="G24" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
       <c r="I24" s="2" t="s">
         <v>39</v>
+      </c>
+      <c r="J24">
+        <v>2</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>39</v>
@@ -3297,8 +3540,14 @@
       <c r="G25" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
       <c r="I25" s="2" t="s">
         <v>39</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>39</v>
@@ -3326,8 +3575,14 @@
       <c r="G26" t="s">
         <v>39</v>
       </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
       <c r="I26" t="s">
         <v>39</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
       </c>
       <c r="K26" t="s">
         <v>39</v>
@@ -3355,8 +3610,14 @@
       <c r="G27" t="s">
         <v>39</v>
       </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
       <c r="I27" t="s">
         <v>39</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
       </c>
       <c r="K27" t="s">
         <v>39</v>
@@ -3384,8 +3645,14 @@
       <c r="G28" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="H28">
+        <v>1.5</v>
+      </c>
       <c r="I28" s="2" t="s">
         <v>39</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>39</v>
@@ -3413,8 +3680,14 @@
       <c r="G29" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
       <c r="I29" s="2" t="s">
         <v>39</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>39</v>
@@ -3442,8 +3715,14 @@
       <c r="G30" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
       <c r="I30" s="2" t="s">
         <v>39</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>39</v>
@@ -3471,8 +3750,14 @@
       <c r="G31" t="s">
         <v>39</v>
       </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
       <c r="I31" t="s">
         <v>39</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
       </c>
       <c r="K31" t="s">
         <v>39</v>
@@ -3520,14 +3805,14 @@
       </c>
       <c r="H33">
         <f>SUM(H4:H31)</f>
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>39</v>
       </c>
       <c r="J33">
         <f>SUM(J4:J31)</f>
-        <v>9.1999999999999993</v>
+        <v>31.5</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>39</v>
@@ -3535,6 +3820,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4084,8 +4370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>